<commit_message>
Modified channelAgc.v to pipeline the enables instead of  waiting for next frame enable. Makes response faster Add FirebirdPll which vco's the clock output to remove the gap. Smooths jitter. Had the clockAndData running on system clock with an enable, but Larry took it out. Removed an asynchronous clock stream.
</commit_message>
<xml_diff>
--- a/DigitalCombiner/SerDes Signal Interconnect.xlsx
+++ b/DigitalCombiner/SerDes Signal Interconnect.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semco\Vivado\Demods\DigitalCombiner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC24DBC-3C16-4BDE-A834-F0FCFD7AAAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B863BF6B-DC13-4997-AC7A-0F276CDBA484}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2790" windowWidth="25455" windowHeight="20880" xr2:uid="{AE219EF2-4569-41BF-838C-D81582E2480E}"/>
+    <workbookView minimized="1" xWindow="5820" yWindow="0" windowWidth="23010" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{AE219EF2-4569-41BF-838C-D81582E2480E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SerDes" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="198">
   <si>
     <t>Ch1</t>
   </si>
@@ -436,6 +446,189 @@
   </si>
   <si>
     <t>NextD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
+  <si>
+    <t>BS_ADC_PwrDn</t>
+  </si>
+  <si>
+    <t>ClkIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsIO_Reset  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsTxEn      </t>
+  </si>
+  <si>
+    <t>BS_ADC_LowZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsSyncClk   </t>
+  </si>
+  <si>
+    <t>BS_ADC_CS_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsIO_Update </t>
+  </si>
+  <si>
+    <t>BS_ADC_SClk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsReset     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsCS_n      </t>
+  </si>
+  <si>
+    <t>BS_ADC_SDIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsSClk      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_ADC_SE  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsMosi      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsMiso      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsPdClk     </t>
+  </si>
+  <si>
+    <t>DdsData17</t>
+  </si>
+  <si>
+    <t>DdsData16</t>
+  </si>
+  <si>
+    <t>DdsData15</t>
+  </si>
+  <si>
+    <t>DdsData14</t>
+  </si>
+  <si>
+    <t>DdsData13</t>
+  </si>
+  <si>
+    <t>DdsData12</t>
+  </si>
+  <si>
+    <t>DdsData11</t>
+  </si>
+  <si>
+    <t>DdsData10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DdsData0 </t>
+  </si>
+  <si>
+    <t>BS_Ovf</t>
+  </si>
+  <si>
+    <t>BS_D13</t>
+  </si>
+  <si>
+    <t>BS_D12</t>
+  </si>
+  <si>
+    <t>BS_D11</t>
+  </si>
+  <si>
+    <t>BS_D10</t>
+  </si>
+  <si>
+    <t>BS_D9</t>
+  </si>
+  <si>
+    <t>BS_D8</t>
+  </si>
+  <si>
+    <t>BS_D7</t>
+  </si>
+  <si>
+    <t>BS_D6</t>
+  </si>
+  <si>
+    <t>BS_D5</t>
+  </si>
+  <si>
+    <t>BS_D4</t>
+  </si>
+  <si>
+    <t>BS_D3</t>
+  </si>
+  <si>
+    <t>BS_D2</t>
+  </si>
+  <si>
+    <t>BS_D1</t>
+  </si>
+  <si>
+    <t>BS_D0</t>
+  </si>
+  <si>
+    <t>IF/BS_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_DAC_SClk] </t>
+  </si>
+  <si>
+    <t>BS_DAC_Sel_n]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_I2C_SCl]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_I2C_SDa]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_PllOut]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_RefPll]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_Clk]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_DAC_MOSI] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_Ovf]      </t>
   </si>
 </sst>
 </file>
@@ -813,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223E953A-C769-4A3C-A208-F4E2D98D14F1}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
@@ -1863,4 +2056,354 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F46C0A8-A468-46FA-9494-365DC07A1806}">
+  <dimension ref="A3:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" t="s">
+        <v>154</v>
+      </c>
+      <c r="G28" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D13">
+    <sortCondition ref="B3:B13"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added mods for NGR filter selects and 50 Ohm terminations
</commit_message>
<xml_diff>
--- a/DigitalCombiner/SerDes Signal Interconnect.xlsx
+++ b/DigitalCombiner/SerDes Signal Interconnect.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semco\Vivado\Demods\DigitalCombiner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Semco\Vivado\Demods2016\DigitalCombiner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B863BF6B-DC13-4997-AC7A-0F276CDBA484}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D641DC-C3D7-48F4-B4F8-0732D55F09E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5820" yWindow="0" windowWidth="23010" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{AE219EF2-4569-41BF-838C-D81582E2480E}"/>
+    <workbookView xWindow="26745" yWindow="13695" windowWidth="24135" windowHeight="15600" xr2:uid="{AE219EF2-4569-41BF-838C-D81582E2480E}"/>
   </bookViews>
   <sheets>
     <sheet name="SerDes" sheetId="1" r:id="rId1"/>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223E953A-C769-4A3C-A208-F4E2D98D14F1}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36:L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1413,7 @@
         <v>119</v>
       </c>
       <c r="L20" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>120</v>
       </c>
       <c r="L23" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1522,7 +1522,7 @@
         <v>121</v>
       </c>
       <c r="L25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
         <v>122</v>
       </c>
       <c r="L27" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>106</v>
       </c>
       <c r="L29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
         <v>124</v>
       </c>
       <c r="L32" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1764,7 +1764,7 @@
         <v>103</v>
       </c>
       <c r="L36" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -1825,7 +1825,7 @@
         <v>106</v>
       </c>
       <c r="L39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -1879,7 +1879,7 @@
         <v>106</v>
       </c>
       <c r="L41" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -1937,7 +1937,7 @@
         <v>107</v>
       </c>
       <c r="L44" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -1988,7 +1988,7 @@
         <v>108</v>
       </c>
       <c r="L46" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2046,7 +2046,7 @@
         <v>109</v>
       </c>
       <c r="L49" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2062,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F46C0A8-A468-46FA-9494-365DC07A1806}">
   <dimension ref="A3:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>